<commit_message>
Major Changes to the code
</commit_message>
<xml_diff>
--- a/zf_application/app_views/data_module/view_client/zf_view_global/view_files/data_templates/staff_data_template.xlsx
+++ b/zf_application/app_views/data_module/view_client/zf_view_global/view_files/data_templates/staff_data_template.xlsx
@@ -68,10 +68,10 @@
     <t>School Role</t>
   </si>
   <si>
-    <t>Id  No.</t>
-  </si>
-  <si>
     <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Id  Number</t>
   </si>
 </sst>
 </file>
@@ -402,14 +402,14 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -427,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>5</v>

</xml_diff>